<commit_message>
DB Nonsense Taken Care Of
</commit_message>
<xml_diff>
--- a/CSci130_Project_gradingsheet.xlsx
+++ b/CSci130_Project_gradingsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Picross\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5428D729-5925-4D06-AF5C-201744C8C765}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AB50B99E-DEF5-4539-AB94-3744B7532704}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CSci130_ProjectFall2018" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Part 1</t>
   </si>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,6 +768,9 @@
       <c r="C21">
         <v>3</v>
       </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -779,6 +782,9 @@
       <c r="C22">
         <v>3</v>
       </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -789,6 +795,9 @@
       </c>
       <c r="C23">
         <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>